<commit_message>
add cover, self evaluation
</commit_message>
<xml_diff>
--- a/thesis/self-evaluation-master.xlsx
+++ b/thesis/self-evaluation-master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peilunhsu/Dropbox/PEI/KTH/Courses/Master_Thesis/RISE/Self-Evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peilunhsu/Dropbox/PEI/KTH/Courses/Master_Thesis/RISE/Git/traffic_flow_estimation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C07E1A-5A04-5E40-918B-C13384264915}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73368A22-D297-F040-A898-1AFAEB129286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mall" sheetId="1" r:id="rId1"/>
@@ -268,9 +268,6 @@
     <t>The thesis has valuable and well-recorded experimental results, which match the purpose of the project.</t>
   </si>
   <si>
-    <t>The thesis has a clear description of the background of the project. The goals, problems, and contributions of the project are all well defined. The student also clearly Delimitated the thesis scope.</t>
-  </si>
-  <si>
     <t>The background knowledge of the thesis is introduced. The thesis includes a comprehensive study of the relevant state-of-the-art works in the area. The experiments are also developed following the conclusions of the literature study.</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
     <t>The student actively participated in two students' thesis presentations and raised critical questions about their thesis and presentations. 
 1. Diego Guillen, Self-Learning Methodology for Failure Detection in an Oil- Hydraulic Press: Predictive maintenance, 10.12.2020
 2. Kamil Nasr, Comparison of Popular Data Processing Systems, 06.04.2021</t>
+  </si>
+  <si>
+    <t>The thesis has a clear description of the background of the project. The goals, problems, and contributions of the project are all well defined. The student also clearly delimitated the thesis scope.</t>
   </si>
 </sst>
 </file>
@@ -342,35 +342,42 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF323333"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -643,7 +650,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -753,18 +760,20 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -777,16 +786,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1164,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,10 +1191,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="35" t="s">
         <v>75</v>
       </c>
@@ -1206,7 +1216,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="45" t="s">
         <v>76</v>
       </c>
       <c r="E2" s="21"/>
@@ -1223,11 +1233,11 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="60" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="46" t="s">
         <v>77</v>
       </c>
       <c r="E3" s="22"/>
@@ -1244,15 +1254,15 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -1299,15 +1309,15 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1337,15 +1347,15 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1356,13 +1366,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1373,15 +1383,15 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1392,15 +1402,15 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="6"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1411,14 +1421,14 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="3"/>
@@ -1430,12 +1440,12 @@
     </row>
     <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="5"/>
@@ -1466,15 +1476,15 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
       <c r="I16" s="6"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1504,15 +1514,15 @@
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
       <c r="I18" s="6"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1523,14 +1533,14 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
       <c r="H19" s="5"/>
       <c r="I19" s="6"/>
       <c r="J19" s="3"/>
@@ -1542,12 +1552,12 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
       <c r="J20" s="3"/>
@@ -1623,15 +1633,15 @@
       <c r="O23" s="3"/>
     </row>
     <row r="24" spans="1:15" ht="43" x14ac:dyDescent="0.2">
-      <c r="A24" s="54"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="62" t="s">
-        <v>80</v>
+      <c r="D24" s="63" t="s">
+        <v>95</v>
       </c>
       <c r="E24" s="36"/>
       <c r="F24" s="19"/>
@@ -1650,15 +1660,15 @@
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" ht="85" x14ac:dyDescent="0.2">
-      <c r="A25" s="55"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="62" t="s">
-        <v>81</v>
+      <c r="D25" s="48" t="s">
+        <v>80</v>
       </c>
       <c r="E25" s="36"/>
       <c r="F25" s="19"/>
@@ -1679,15 +1689,15 @@
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="A26" s="55"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="62" t="s">
-        <v>82</v>
+      <c r="D26" s="48" t="s">
+        <v>81</v>
       </c>
       <c r="E26" s="36"/>
       <c r="F26" s="19"/>
@@ -1706,14 +1716,14 @@
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" ht="43" x14ac:dyDescent="0.2">
-      <c r="A27" s="55"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="62" t="s">
+      <c r="D27" s="48" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="36"/>
@@ -1733,15 +1743,15 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" ht="29" x14ac:dyDescent="0.2">
-      <c r="A28" s="55"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="62" t="s">
-        <v>83</v>
+      <c r="D28" s="48" t="s">
+        <v>82</v>
       </c>
       <c r="E28" s="36"/>
       <c r="F28" s="19"/>
@@ -1760,15 +1770,15 @@
       <c r="O28" s="3"/>
     </row>
     <row r="29" spans="1:15" ht="71" x14ac:dyDescent="0.2">
-      <c r="A29" s="55"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="62" t="s">
-        <v>84</v>
+      <c r="D29" s="48" t="s">
+        <v>83</v>
       </c>
       <c r="E29" s="36"/>
       <c r="F29" s="19"/>
@@ -1787,15 +1797,15 @@
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="1:15" ht="71" x14ac:dyDescent="0.2">
-      <c r="A30" s="55"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="62" t="s">
-        <v>85</v>
+      <c r="D30" s="48" t="s">
+        <v>84</v>
       </c>
       <c r="E30" s="36"/>
       <c r="F30" s="19"/>
@@ -1807,22 +1817,22 @@
       </c>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
     </row>
     <row r="31" spans="1:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="A31" s="55"/>
+      <c r="A31" s="57"/>
       <c r="B31" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="62" t="s">
-        <v>86</v>
+      <c r="D31" s="48" t="s">
+        <v>85</v>
       </c>
       <c r="E31" s="36"/>
       <c r="F31" s="19"/>
@@ -1841,22 +1851,22 @@
       <c r="O31" s="3"/>
     </row>
     <row r="32" spans="1:15" ht="113" x14ac:dyDescent="0.2">
-      <c r="A32" s="56"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="62" t="s">
-        <v>87</v>
+      <c r="D32" s="48" t="s">
+        <v>86</v>
       </c>
       <c r="E32" s="36"/>
       <c r="F32" s="25"/>
       <c r="G32" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H32" s="52" t="s">
+      <c r="H32" s="54" t="s">
         <v>65</v>
       </c>
       <c r="I32" s="11"/>
@@ -1875,7 +1885,7 @@
       <c r="E33" s="37"/>
       <c r="F33" s="12"/>
       <c r="G33" s="27"/>
-      <c r="H33" s="53"/>
+      <c r="H33" s="55"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
@@ -1885,7 +1895,7 @@
       <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" ht="85" x14ac:dyDescent="0.2">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="56" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1894,15 +1904,15 @@
       <c r="C34" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="62" t="s">
-        <v>88</v>
+      <c r="D34" s="48" t="s">
+        <v>87</v>
       </c>
       <c r="E34" s="36"/>
       <c r="F34" s="25"/>
       <c r="G34" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="53"/>
+      <c r="H34" s="55"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
@@ -1912,22 +1922,22 @@
       <c r="O34" s="3"/>
     </row>
     <row r="35" spans="1:15" ht="71" x14ac:dyDescent="0.2">
-      <c r="A35" s="55"/>
+      <c r="A35" s="57"/>
       <c r="B35" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="62" t="s">
-        <v>89</v>
+      <c r="D35" s="48" t="s">
+        <v>88</v>
       </c>
       <c r="E35" s="36"/>
       <c r="F35" s="25"/>
       <c r="G35" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="53"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
@@ -1937,22 +1947,22 @@
       <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15" ht="43" x14ac:dyDescent="0.2">
-      <c r="A36" s="55"/>
+      <c r="A36" s="57"/>
       <c r="B36" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="62" t="s">
-        <v>90</v>
+      <c r="D36" s="48" t="s">
+        <v>89</v>
       </c>
       <c r="E36" s="36"/>
       <c r="F36" s="25"/>
       <c r="G36" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H36" s="53"/>
+      <c r="H36" s="55"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
@@ -1962,22 +1972,22 @@
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="A37" s="56"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="62" t="s">
-        <v>91</v>
+      <c r="D37" s="48" t="s">
+        <v>90</v>
       </c>
       <c r="E37" s="36"/>
       <c r="F37" s="25"/>
       <c r="G37" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H37" s="53"/>
+      <c r="H37" s="55"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
@@ -2004,7 +2014,7 @@
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" ht="43" x14ac:dyDescent="0.2">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="56" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="8" t="s">
@@ -2013,8 +2023,8 @@
       <c r="C39" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="62" t="s">
-        <v>92</v>
+      <c r="D39" s="48" t="s">
+        <v>91</v>
       </c>
       <c r="E39" s="36"/>
       <c r="F39" s="19"/>
@@ -2033,15 +2043,15 @@
       <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" ht="71" x14ac:dyDescent="0.2">
-      <c r="A40" s="55"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="62" t="s">
-        <v>93</v>
+      <c r="D40" s="48" t="s">
+        <v>92</v>
       </c>
       <c r="E40" s="36"/>
       <c r="F40" s="19"/>
@@ -2060,15 +2070,15 @@
       <c r="O40" s="3"/>
     </row>
     <row r="41" spans="1:15" ht="57" x14ac:dyDescent="0.2">
-      <c r="A41" s="55"/>
+      <c r="A41" s="57"/>
       <c r="B41" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="62" t="s">
-        <v>94</v>
+      <c r="D41" s="48" t="s">
+        <v>93</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="19"/>
@@ -2087,15 +2097,15 @@
       <c r="O41" s="3"/>
     </row>
     <row r="42" spans="1:15" ht="99" x14ac:dyDescent="0.2">
-      <c r="A42" s="56"/>
+      <c r="A42" s="58"/>
       <c r="B42" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="62" t="s">
-        <v>95</v>
+      <c r="D42" s="48" t="s">
+        <v>94</v>
       </c>
       <c r="E42" s="36"/>
       <c r="F42" s="19"/>
@@ -2131,10 +2141,10 @@
       <c r="O43" s="3"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="50"/>
       <c r="C44" s="3"/>
       <c r="D44" s="7" t="s">
         <v>5</v>
@@ -2349,12 +2359,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:G19"/>
     <mergeCell ref="K30:O30"/>
     <mergeCell ref="H32:H37"/>
     <mergeCell ref="A34:A37"/>
@@ -2364,11 +2373,12 @@
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C24:C32 C34:C37 C39:C42" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>